<commit_message>
short names and variable for "clean_name" used in most maps or summary tables. Merges with agency_name or agency_number in assessor data
</commit_message>
<xml_diff>
--- a/muni_shortnames.xlsx
+++ b/muni_shortnames.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B1E18-57BE-421F-B216-99C4FEDADC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0520A2AA-151B-4DD7-B36C-5E070ADD84DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{E04B2839-4174-4D46-99FA-03AE29BCB57B}"/>
+    <workbookView xWindow="15960" yWindow="-16200" windowWidth="14400" windowHeight="14985" xr2:uid="{E04B2839-4174-4D46-99FA-03AE29BCB57B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="17" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="436">
   <si>
     <t>VILLAGE OF ALSIP</t>
   </si>
@@ -1338,6 +1342,12 @@
   </si>
   <si>
     <t>Most recent reassessed</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Average of Most recent reassessed</t>
   </si>
 </sst>
 </file>
@@ -1415,7 +1425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1423,37 +1433,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0"/>
-        <name val="Times New Roman"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1575,6 +1566,30 @@
         </left>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="0"/>
+        <name val="Times New Roman"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1588,21 +1603,2848 @@
 </styleSheet>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alea Wilbur" refreshedDate="45183.474098726852" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="134" xr:uid="{96453F7C-CC08-4E98-8CEC-506741AA0D86}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="agency_number" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="20060000" maxValue="31350000"/>
+    </cacheField>
+    <cacheField name="agency_name" numFmtId="0">
+      <sharedItems count="134">
+        <s v="CITY OF CHICAGO"/>
+        <s v="VILLAGE OF BARRINGTON"/>
+        <s v="VILLAGE OF BARRINGTON HILLS"/>
+        <s v="VILLAGE OF EAST DUNDEE"/>
+        <s v="VILLAGE OF SOUTH BARRINGTON"/>
+        <s v="VILLAGE OF ELK GROVE VILLAGE"/>
+        <s v="VILLAGE OF MT PROSPECT"/>
+        <s v="CITY OF EVANSTON"/>
+        <s v="CITY OF NORTH LAKE"/>
+        <s v="VILLAGE OF BENSENVILLE"/>
+        <s v="VILLAGE OF ELMWOOD PARK"/>
+        <s v="VILLAGE OF FRANKLIN PARK"/>
+        <s v="VILLAGE OF RIVER GROVE"/>
+        <s v="VILLAGE OF SCHILLER PARK"/>
+        <s v="CITY OF DES PLAINES"/>
+        <s v="CITY OF PARK RIDGE"/>
+        <s v="VILLAGE OF ROSEMONT"/>
+        <s v="VILLAGE OF GLENCOE"/>
+        <s v="VILLAGE OF KENILWORTH"/>
+        <s v="VILLAGE OF WILMETTE"/>
+        <s v="VILLAGE OF WINNETKA"/>
+        <s v="VILLAGE OF GOLF"/>
+        <s v="VILLAGE OF LINCOLNWOOD"/>
+        <s v="VILLAGE OF MORTON GROVE"/>
+        <s v="VILLAGE OF NILES"/>
+        <s v="VILLAGE OF SKOKIE"/>
+        <s v="VILLAGE OF DEERFIELD"/>
+        <s v="VILLAGE OF GLENVIEW"/>
+        <s v="VILLAGE OF NORTHBROOK"/>
+        <s v="VILLAGE OF NORTHFIELD"/>
+        <s v="VILLAGE OF OAK BROOK"/>
+        <s v="VILLAGE OF HARWOOD HEIGHTS"/>
+        <s v="VILLAGE OF NORRIDGE"/>
+        <s v="CITY OF ROLLING MEADOWS"/>
+        <s v="VILLAGE OF DEER PARK"/>
+        <s v="VILLAGE OF INVERNESS"/>
+        <s v="VILLAGE OF PALATINE"/>
+        <s v="VILLAGE OF HOFFMAN ESTATES"/>
+        <s v="VILLAGE OF ROSELLE"/>
+        <s v="VILLAGE OF SCHAUMBURG"/>
+        <s v="CITY OF PROSPECT HEIGHTS"/>
+        <s v="VILLAGE OF ARLINGTON HEIGHTS"/>
+        <s v="VILLAGE OF BUFFALO GROVE"/>
+        <s v="VILLAGE OF WHEELING"/>
+        <s v="CITY OF BERWYN"/>
+        <s v="CITY OF CHICAGO HEIGHTS"/>
+        <s v="VILLAGE OF FORD HEIGHTS"/>
+        <s v="VILLAGE OF GLENWOOD"/>
+        <s v="VILLAGE OF LYNWOOD"/>
+        <s v="VILLAGE OF SAUK VILLAGE"/>
+        <s v="VILLAGE OF SOUTH CHICAGO HEIGHTS"/>
+        <s v="VILLAGE OF STEGER"/>
+        <s v="CITY OF COUNTRY CLUB HILLS"/>
+        <s v="CITY OF MARKHAM"/>
+        <s v="CITY OF OAK FOREST"/>
+        <s v="VILLAGE OF CRESTWOOD"/>
+        <s v="VILLAGE OF HAZELCREST"/>
+        <s v="VILLAGE OF MIDLOTHIAN"/>
+        <s v="VILLAGE OF POSEN"/>
+        <s v="VILLAGE OF ROBBINS"/>
+        <s v="VILLAGE OF TINLEY PARK"/>
+        <s v="CITY OF BLUE ISLAND"/>
+        <s v="VILLAGE OF CALUMET PARK"/>
+        <s v="TOWN CICERO"/>
+        <s v="CITY OF ELGIN"/>
+        <s v="VILLAGE OF BARTLETT"/>
+        <s v="VILLAGE OF STREAMWOOD"/>
+        <s v="VILLAGE OF LEMONT"/>
+        <s v="CITY OF COUNTRYSIDE"/>
+        <s v="VILLAGE OF BRIDGEVIEW"/>
+        <s v="VILLAGE OF BURR RIDGE"/>
+        <s v="VILLAGE OF HANOVER PARK"/>
+        <s v="VILLAGE OF HINSDALE"/>
+        <s v="VILLAGE OF HODGKINS"/>
+        <s v="VILLAGE OF HOMER GLEN"/>
+        <s v="VILLAGE OF INDIAN HEAD PARK"/>
+        <s v="VILLAGE OF JUSTICE"/>
+        <s v="VILLAGE OF LA GRANGE"/>
+        <s v="VILLAGE OF LA GRANGE PARK"/>
+        <s v="VILLAGE OF LYONS"/>
+        <s v="VILLAGE OF MC COOK"/>
+        <s v="VILLAGE OF SUMMIT"/>
+        <s v="VILLAGE OF WESTERN SPRINGS"/>
+        <s v="VILLAGE OF WILLOW SPRINGS"/>
+        <s v="VILLAGE OF OAK PARK"/>
+        <s v="VILLAGE OF ORLAND HILLS"/>
+        <s v="VILLAGE OF ORLAND PARK"/>
+        <s v="CITY OF HICKORY HILLS"/>
+        <s v="CITY OF PALOS HEIGHTS"/>
+        <s v="CITY OF PALOS HILLS"/>
+        <s v="VILLAGE OF PALOS PARK"/>
+        <s v="VILLAGE OF BELLWOOD"/>
+        <s v="VILLAGE OF BERKELEY"/>
+        <s v="VILLAGE OF BROADVIEW"/>
+        <s v="VILLAGE OF BROOKFIELD"/>
+        <s v="VILLAGE OF FOREST PARK"/>
+        <s v="VILLAGE OF HILLSIDE"/>
+        <s v="VILLAGE OF MAYWOOD"/>
+        <s v="VILLAGE OF MELROSE PARK"/>
+        <s v="VILLAGE OF STONE PARK"/>
+        <s v="VILLAGE OF WESTCHESTER"/>
+        <s v="VILLAGE OF FLOSSMOOR"/>
+        <s v="VILLAGE OF FRANKFORT"/>
+        <s v="VILLAGE OF MATTESON"/>
+        <s v="VILLAGE OF OLYMPIA FIELDS"/>
+        <s v="VILLAGE OF PARK FOREST"/>
+        <s v="VILLAGE OF RICHTON PARK"/>
+        <s v="VILLAGE OF UNIVERSITY PARK"/>
+        <s v="VILLAGE OF RIVER FOREST"/>
+        <s v="VILLAGE OF NORTH RIVERSIDE"/>
+        <s v="VILLAGE OF RIVERSIDE"/>
+        <s v="CITY OF BURBANK"/>
+        <s v="VILLAGE OF BEDFORD PARK"/>
+        <s v="VILLAGE OF FORESTVIEW"/>
+        <s v="VILLAGE OF STICKNEY"/>
+        <s v="CITY OF CALUMET CITY"/>
+        <s v="CITY OF HARVEY"/>
+        <s v="VILLAGE OF BURNHAM"/>
+        <s v="VILLAGE OF DIXMOOR"/>
+        <s v="VILLAGE OF DOLTON"/>
+        <s v="VILLAGE OF EAST HAZELCREST"/>
+        <s v="VILLAGE OF HOMEWOOD"/>
+        <s v="VILLAGE OF LANSING"/>
+        <s v="VILLAGE OF PHOENIX"/>
+        <s v="VILLAGE OF RIVERDALE"/>
+        <s v="VILLAGE OF SOUTH HOLLAND"/>
+        <s v="VILLAGE OF THORNTON"/>
+        <s v="CITY OF HOMETOWN"/>
+        <s v="VILLAGE OF ALSIP"/>
+        <s v="VILLAGE OF CHICAGO RIDGE"/>
+        <s v="VILLAGE OF EVERGREEN PARK"/>
+        <s v="VILLAGE OF MERRIONETTE PARK"/>
+        <s v="VILLAGE OF OAK LAWN"/>
+        <s v="VILLAGE OF WORTH"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="short_name" numFmtId="0">
+      <sharedItems count="133">
+        <s v="CHICAGO"/>
+        <s v="BARRINGTON"/>
+        <s v="BARRINGTON HILLS"/>
+        <s v="EAST DUNDEE"/>
+        <s v="SOUTH BARRINGTON"/>
+        <s v="ELK GROVE VILLAGE"/>
+        <s v="MT PROSPECT"/>
+        <s v="EVANSTON"/>
+        <s v="NORTH LAKE"/>
+        <s v="BENSENVILLE"/>
+        <s v="ELMWOOD PARK"/>
+        <s v="FRANKLIN PARK"/>
+        <s v="RIVER GROVE"/>
+        <s v="SCHILLER PARK"/>
+        <s v="DES PLAINES"/>
+        <s v="PARK RIDGE"/>
+        <s v="ROSEMONT"/>
+        <s v="GLENCOE"/>
+        <s v="KENILWORTH"/>
+        <s v="WILMETTE"/>
+        <s v="WINNETKA"/>
+        <s v="GOLF"/>
+        <s v="LINCOLNWOOD"/>
+        <s v="MORTON GROVE"/>
+        <s v="NILES"/>
+        <s v="SKOKIE"/>
+        <s v="DEERFIELD"/>
+        <s v="GLENVIEW"/>
+        <s v="NORTHBROOK"/>
+        <s v="NORTHFIELD"/>
+        <s v="OAK BROOK"/>
+        <s v="HARWOOD HEIGHTS"/>
+        <s v="NORRIDGE"/>
+        <s v="ROLLING MEADOWS"/>
+        <s v="DEER PARK"/>
+        <s v="INVERNESS"/>
+        <s v="PALATINE"/>
+        <s v="HOFFMAN ESTATES"/>
+        <s v="ROSELLE"/>
+        <s v="SCHAUMBURG"/>
+        <s v="PROSPECT HEIGHTS"/>
+        <s v="ARLINGTON HEIGHTS"/>
+        <s v="BUFFALO GROVE"/>
+        <s v="WHEELING"/>
+        <s v="BERWYN"/>
+        <s v="CHICAGO HEIGHTS"/>
+        <s v="FORD HEIGHTS"/>
+        <s v="GLENWOOD"/>
+        <s v="LYNWOOD"/>
+        <s v="SAUK VILLAGE"/>
+        <s v="SOUTH CHICAGO HEIGHTS"/>
+        <s v="STEGER"/>
+        <s v="COUNTRY CLUB HILLS"/>
+        <s v="MARKHAM"/>
+        <s v="OAK FOREST"/>
+        <s v="CRESTWOOD"/>
+        <s v="HAZELCREST"/>
+        <s v="MIDLOTHIAN"/>
+        <s v="POSEN"/>
+        <s v="ROBBINS"/>
+        <s v="TINLEY PARK"/>
+        <s v="BLUE ISLAND"/>
+        <s v="CALUMET PARK"/>
+        <s v="CICERO"/>
+        <s v="ELGIN"/>
+        <s v="BARTLETT"/>
+        <s v="STREAMWOOD"/>
+        <s v="LEMONT"/>
+        <s v="COUNTRYSIDE"/>
+        <s v="BRIDGEVIEW"/>
+        <s v="BURR RIDGE"/>
+        <s v="HANOVER PARK"/>
+        <s v="HINSDALE"/>
+        <s v="HODGKINS"/>
+        <s v="HOMER GLEN"/>
+        <s v="INDIAN HEAD PARK"/>
+        <s v="JUSTICE"/>
+        <s v="LA GRANGE"/>
+        <s v="LA GRANGE PARK"/>
+        <s v="LYONS"/>
+        <s v="MC COOK"/>
+        <s v="SUMMIT"/>
+        <s v="WESTERN SPRINGS"/>
+        <s v="WILLOW SPRINGS"/>
+        <s v="OAK PARK"/>
+        <s v="ORLAND HILLS"/>
+        <s v="ORLAND PARK"/>
+        <s v="HICKORY HILLS"/>
+        <s v="PALOS HEIGHTS"/>
+        <s v="PALOS HILLS"/>
+        <s v="PALOS PARK"/>
+        <s v="BELLWOOD"/>
+        <s v="BERKELEY"/>
+        <s v="BROADVIEW"/>
+        <s v="BROOKFIELD"/>
+        <s v="FOREST PARK"/>
+        <s v="HILLSIDE"/>
+        <s v="MAYWOOD"/>
+        <s v="MELROSE PARK"/>
+        <s v="STONE PARK"/>
+        <s v="WESTCHESTER"/>
+        <s v="FLOSSMOOR"/>
+        <s v="FRANKFORT"/>
+        <s v="MATTESON"/>
+        <s v="OLYMPIA FIELDS"/>
+        <s v="PARK FOREST"/>
+        <s v="RICHTON PARK"/>
+        <s v="UNIVERSITY PARK"/>
+        <s v="RIVER FOREST"/>
+        <s v="NORTH RIVERSIDE"/>
+        <s v="RIVERSIDE"/>
+        <s v="BURBANK"/>
+        <s v="BEDFORD PARK"/>
+        <s v="FORESTVIEW"/>
+        <s v="STICKNEY"/>
+        <s v="CALUMET CITY"/>
+        <s v="HARVEY"/>
+        <s v="BURNHAM"/>
+        <s v="DIXMOOR"/>
+        <s v="DOLTON"/>
+        <s v="EAST HAZELCREST"/>
+        <s v="HOMEWOOD"/>
+        <s v="LANSING"/>
+        <s v="PHOENIX"/>
+        <s v="RIVERDALE"/>
+        <s v="SOUTH HOLLAND"/>
+        <s v="THORNTON"/>
+        <s v="HOMETOWN"/>
+        <s v="ALSIP"/>
+        <s v="CHICAGO RIDGE"/>
+        <s v="EVERGREEN PARK"/>
+        <s v="MERRIONETTE PARK"/>
+        <s v="OAK LAWN"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="clean_name" numFmtId="0">
+      <sharedItems count="134">
+        <s v="Chicago"/>
+        <s v="Barrington"/>
+        <s v="Barrington Hills"/>
+        <s v="East Dundee"/>
+        <s v="South Barrington"/>
+        <s v="Elk Grove Village"/>
+        <s v="Mt Prospect"/>
+        <s v="Evanston"/>
+        <s v="North Lake"/>
+        <s v="Bensenville"/>
+        <s v="Elmwood Park"/>
+        <s v="Franklin Park"/>
+        <s v="River Grove"/>
+        <s v="Schiller Park"/>
+        <s v="Des Plaines"/>
+        <s v="Park Ridge"/>
+        <s v="Rosemont"/>
+        <s v="Glencoe"/>
+        <s v="Kenilworth"/>
+        <s v="Wilmette"/>
+        <s v="Winnetka"/>
+        <s v="Golf"/>
+        <s v="Lincolnwood"/>
+        <s v="Morton Grove"/>
+        <s v="Niles"/>
+        <s v="Skokie"/>
+        <s v="Deerfield"/>
+        <s v="Glenview"/>
+        <s v="Northbrook"/>
+        <s v="Northfield"/>
+        <s v="Oak Brook"/>
+        <s v="Harwood Heights"/>
+        <s v="Norridge"/>
+        <s v="Rolling Meadows"/>
+        <s v="Deer Park"/>
+        <s v="Inverness"/>
+        <s v="Palatine"/>
+        <s v="Hoffman Estates"/>
+        <s v="Roselle"/>
+        <s v="Schaumburg"/>
+        <s v="Prospect Heights"/>
+        <s v="Arlington Heights"/>
+        <s v="Buffalo Grove"/>
+        <s v="Wheeling"/>
+        <s v="Berwyn"/>
+        <s v="Chicago Heights"/>
+        <s v="Ford Heights"/>
+        <s v="Glenwood"/>
+        <s v="Lynwood"/>
+        <s v="Sauk Village"/>
+        <s v="South Chicago Heights"/>
+        <s v="Steger"/>
+        <s v="Country Club Hills"/>
+        <s v="Markham"/>
+        <s v="Oak Forest"/>
+        <s v="Crestwood"/>
+        <s v="Hazelcrest"/>
+        <s v="Midlothian"/>
+        <s v="Posen"/>
+        <s v="Robbins"/>
+        <s v="Tinley Park"/>
+        <s v="Blue Island"/>
+        <s v="Calumet Park"/>
+        <s v="Cicero"/>
+        <s v="Elgin"/>
+        <s v="Bartlett"/>
+        <s v="Streamwood"/>
+        <s v="Lemont"/>
+        <s v="Countryside"/>
+        <s v="Bridgeview"/>
+        <s v="Burr Ridge"/>
+        <s v="Hanover Park"/>
+        <s v="Hinsdale"/>
+        <s v="Hodgkins"/>
+        <s v="Homer Glen"/>
+        <s v="Indian Head Park"/>
+        <s v="Justice"/>
+        <s v="La Grange"/>
+        <s v="La Grange Park"/>
+        <s v="Lyons"/>
+        <s v="Mc Cook"/>
+        <s v="Summit"/>
+        <s v="Western Springs"/>
+        <s v="Willow Springs"/>
+        <s v="Oak Park"/>
+        <s v="Orland Hills"/>
+        <s v="Orland Park"/>
+        <s v="Hickory Hills"/>
+        <s v="Palos Heights"/>
+        <s v="Palos Hills"/>
+        <s v="Palos Park"/>
+        <s v="Bellwood"/>
+        <s v="Berkeley"/>
+        <s v="Broadview"/>
+        <s v="Brookfield"/>
+        <s v="Forest Park"/>
+        <s v="Hillside"/>
+        <s v="Maywood"/>
+        <s v="Melrose Park"/>
+        <s v="Stone Park"/>
+        <s v="Westchester"/>
+        <s v="Flossmoor"/>
+        <s v="Frankfort"/>
+        <s v="Matteson"/>
+        <s v="Olympia Fields"/>
+        <s v="Park Forest"/>
+        <s v="Richton Park"/>
+        <s v="University Park"/>
+        <s v="River Forest"/>
+        <s v="North Riverside"/>
+        <s v="Riverside"/>
+        <s v="Burbank"/>
+        <s v="Bedford Park"/>
+        <s v="Forestview"/>
+        <s v="Stickney"/>
+        <s v="Calumet City"/>
+        <s v="Harvey"/>
+        <s v="Burnham"/>
+        <s v="Dixmoor"/>
+        <s v="Dolton"/>
+        <s v="East Hazelcrest"/>
+        <s v="Homewood"/>
+        <s v="Lansing"/>
+        <s v="Phoenix"/>
+        <s v="Riverdale"/>
+        <s v="South Holland"/>
+        <s v="Thornton"/>
+        <s v="Hometown"/>
+        <s v="Alsip"/>
+        <s v="Chicago Ridge"/>
+        <s v="Evergreen Park"/>
+        <s v="Merrionette Park"/>
+        <s v="Oak Lawn"/>
+        <s v="Worth"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="shpfile_name" numFmtId="0">
+      <sharedItems count="134">
+        <s v="Chicago"/>
+        <s v="Barrington"/>
+        <s v="Barrington Hills"/>
+        <s v="East Dundee"/>
+        <s v="South Barrington"/>
+        <s v="Elk Grove Village"/>
+        <s v="Mount Prospect"/>
+        <s v="Evanston"/>
+        <s v="Northlake"/>
+        <s v="Bensenville"/>
+        <s v="Elmwood Park"/>
+        <s v="Franklin Park"/>
+        <s v="River Grove"/>
+        <s v="Schiller Park"/>
+        <s v="Des Plaines"/>
+        <s v="Park Ridge"/>
+        <s v="Rosemont"/>
+        <s v="Glencoe"/>
+        <s v="Kenilworth"/>
+        <s v="Wilmette"/>
+        <s v="Winnetka"/>
+        <s v="Golf"/>
+        <s v="Lincolnwood"/>
+        <s v="Morton Grove"/>
+        <s v="Niles"/>
+        <s v="Skokie"/>
+        <s v="Deerfield"/>
+        <s v="Glenview"/>
+        <s v="Northbrook"/>
+        <s v="Northfield"/>
+        <s v="Oak Brook"/>
+        <s v="Harwood Heights"/>
+        <s v="Norridge"/>
+        <s v="Rolling Meadows"/>
+        <s v="Deer Park"/>
+        <s v="Inverness"/>
+        <s v="Palatine"/>
+        <s v="Hoffman Estates"/>
+        <s v="Roselle"/>
+        <s v="Schaumburg"/>
+        <s v="Prospect Heights"/>
+        <s v="Arlington Heights"/>
+        <s v="Buffalo Grove"/>
+        <s v="Wheeling"/>
+        <s v="Berwyn"/>
+        <s v="Chicago Heights"/>
+        <s v="Ford Heights"/>
+        <s v="Glenwood"/>
+        <s v="Lynwood"/>
+        <s v="Sauk Village"/>
+        <s v="South Chicago Heights"/>
+        <s v="Steger"/>
+        <s v="Country Club Hills"/>
+        <s v="Markham"/>
+        <s v="Oak Forest"/>
+        <s v="Crestwood"/>
+        <s v="Hazel Crest"/>
+        <s v="Midlothian"/>
+        <s v="Posen"/>
+        <s v="Robbins"/>
+        <s v="Tinley Park"/>
+        <s v="Blue Island"/>
+        <s v="Calumet Park"/>
+        <s v="Cicero"/>
+        <s v="Elgin"/>
+        <s v="Bartlett"/>
+        <s v="Streamwood"/>
+        <s v="Lemont"/>
+        <s v="Countryside"/>
+        <s v="Bridgeview"/>
+        <s v="Burr Ridge"/>
+        <s v="Hanover Park"/>
+        <s v="Hinsdale"/>
+        <s v="Hodgkins"/>
+        <s v="Homer Glen"/>
+        <s v="Indian Head Park"/>
+        <s v="Justice"/>
+        <s v="La Grange"/>
+        <s v="La Grange Park"/>
+        <s v="Lyons"/>
+        <s v="Mc Cook"/>
+        <s v="Summit"/>
+        <s v="Western Springs"/>
+        <s v="Willow Springs"/>
+        <s v="Oak Park"/>
+        <s v="Orland Hills"/>
+        <s v="Orland Park"/>
+        <s v="Hickory Hills"/>
+        <s v="Palos Heights"/>
+        <s v="Palos Hills"/>
+        <s v="Palos Park"/>
+        <s v="Bellwood"/>
+        <s v="Berkeley"/>
+        <s v="Broadview"/>
+        <s v="Brookfield"/>
+        <s v="Forest Park"/>
+        <s v="Hillside"/>
+        <s v="Maywood"/>
+        <s v="Melrose Park"/>
+        <s v="Stone Park"/>
+        <s v="Westchester"/>
+        <s v="Flossmoor"/>
+        <s v="Frankfort"/>
+        <s v="Matteson"/>
+        <s v="Olympia Fields"/>
+        <s v="Park Forest"/>
+        <s v="Richton Park"/>
+        <s v="University Park"/>
+        <s v="River Forest"/>
+        <s v="North Riverside"/>
+        <s v="Riverside"/>
+        <s v="Burbank"/>
+        <s v="Bedford Park"/>
+        <s v="Forest View"/>
+        <s v="Stickney"/>
+        <s v="Calumet City"/>
+        <s v="Harvey"/>
+        <s v="Burnham"/>
+        <s v="Dixmoor"/>
+        <s v="Dolton"/>
+        <s v="East Hazel Crest"/>
+        <s v="Homewood"/>
+        <s v="Lansing"/>
+        <s v="Phoenix"/>
+        <s v="Riverdale"/>
+        <s v="South Holland"/>
+        <s v="Thornton"/>
+        <s v="Hometown"/>
+        <s v="Alsip"/>
+        <s v="Chicago Ridge"/>
+        <s v="Evergreen Park"/>
+        <s v="Merrionette Park"/>
+        <s v="Oak Lawn"/>
+        <s v="Worth"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Triad" numFmtId="0">
+      <sharedItems count="3">
+        <s v="City"/>
+        <s v="North"/>
+        <s v="South"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Township" numFmtId="0">
+      <sharedItems count="31">
+        <s v="Chicago"/>
+        <s v="Barrington"/>
+        <s v="Elk Grove"/>
+        <s v="Evanston"/>
+        <s v="Leyden"/>
+        <s v="Maine"/>
+        <s v="New Trier"/>
+        <s v="Niles"/>
+        <s v="Northfield"/>
+        <s v="Norwood Park"/>
+        <s v="Palatine"/>
+        <s v="Schaumburg"/>
+        <s v="Wheeling"/>
+        <s v="Berwyn"/>
+        <s v="Bloom"/>
+        <s v="Bremen"/>
+        <s v="Calumet"/>
+        <s v="Cicero"/>
+        <s v="Hanover"/>
+        <s v="Lemont"/>
+        <s v="Lyons"/>
+        <s v="Oak Park"/>
+        <s v="Orland"/>
+        <s v="Palos"/>
+        <s v="Proviso"/>
+        <s v="Rich"/>
+        <s v="River Forest"/>
+        <s v="Riverside"/>
+        <s v="Stickney"/>
+        <s v="Thornton"/>
+        <s v="Worth"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Column1" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Most recent reassessed" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2021"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="134">
+  <r>
+    <n v="30210000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="2021"/>
+  </r>
+  <r>
+    <n v="30030000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30040000"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30320000"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31180000"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30350000"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="2"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30820000"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Wheeling"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30380000"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30850000"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="4"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30080000"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30370000"/>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="4"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30450000"/>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="4"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31070000"/>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="4"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31160000"/>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="4"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30290000"/>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31010000"/>
+    <x v="15"/>
+    <x v="15"/>
+    <x v="15"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31130000"/>
+    <x v="16"/>
+    <x v="16"/>
+    <x v="16"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Leydon"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30460000"/>
+    <x v="17"/>
+    <x v="17"/>
+    <x v="17"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="6"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30650000"/>
+    <x v="18"/>
+    <x v="18"/>
+    <x v="18"/>
+    <x v="18"/>
+    <x v="1"/>
+    <x v="6"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31330000"/>
+    <x v="19"/>
+    <x v="19"/>
+    <x v="19"/>
+    <x v="19"/>
+    <x v="1"/>
+    <x v="6"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31340000"/>
+    <x v="20"/>
+    <x v="20"/>
+    <x v="20"/>
+    <x v="20"/>
+    <x v="1"/>
+    <x v="6"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30490000"/>
+    <x v="21"/>
+    <x v="21"/>
+    <x v="21"/>
+    <x v="21"/>
+    <x v="1"/>
+    <x v="7"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30700000"/>
+    <x v="22"/>
+    <x v="22"/>
+    <x v="22"/>
+    <x v="22"/>
+    <x v="1"/>
+    <x v="7"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30810000"/>
+    <x v="23"/>
+    <x v="23"/>
+    <x v="23"/>
+    <x v="23"/>
+    <x v="1"/>
+    <x v="7"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30830000"/>
+    <x v="24"/>
+    <x v="24"/>
+    <x v="24"/>
+    <x v="24"/>
+    <x v="1"/>
+    <x v="7"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31170000"/>
+    <x v="25"/>
+    <x v="25"/>
+    <x v="25"/>
+    <x v="25"/>
+    <x v="1"/>
+    <x v="7"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30280000"/>
+    <x v="26"/>
+    <x v="26"/>
+    <x v="26"/>
+    <x v="26"/>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30470000"/>
+    <x v="27"/>
+    <x v="27"/>
+    <x v="27"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="8"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30870000"/>
+    <x v="28"/>
+    <x v="28"/>
+    <x v="28"/>
+    <x v="28"/>
+    <x v="1"/>
+    <x v="8"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30880000"/>
+    <x v="29"/>
+    <x v="29"/>
+    <x v="29"/>
+    <x v="29"/>
+    <x v="1"/>
+    <x v="8"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30890000"/>
+    <x v="30"/>
+    <x v="30"/>
+    <x v="30"/>
+    <x v="30"/>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30520000"/>
+    <x v="31"/>
+    <x v="31"/>
+    <x v="31"/>
+    <x v="31"/>
+    <x v="1"/>
+    <x v="9"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30840000"/>
+    <x v="32"/>
+    <x v="32"/>
+    <x v="32"/>
+    <x v="32"/>
+    <x v="1"/>
+    <x v="9"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31110000"/>
+    <x v="33"/>
+    <x v="33"/>
+    <x v="33"/>
+    <x v="33"/>
+    <x v="1"/>
+    <x v="10"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30270000"/>
+    <x v="34"/>
+    <x v="34"/>
+    <x v="34"/>
+    <x v="34"/>
+    <x v="1"/>
+    <x v="10"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30630000"/>
+    <x v="35"/>
+    <x v="35"/>
+    <x v="35"/>
+    <x v="35"/>
+    <x v="1"/>
+    <x v="10"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30960000"/>
+    <x v="36"/>
+    <x v="36"/>
+    <x v="36"/>
+    <x v="36"/>
+    <x v="1"/>
+    <x v="10"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30580000"/>
+    <x v="37"/>
+    <x v="37"/>
+    <x v="37"/>
+    <x v="37"/>
+    <x v="1"/>
+    <x v="11"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31120000"/>
+    <x v="38"/>
+    <x v="38"/>
+    <x v="38"/>
+    <x v="38"/>
+    <x v="1"/>
+    <x v="11"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31150000"/>
+    <x v="39"/>
+    <x v="39"/>
+    <x v="39"/>
+    <x v="39"/>
+    <x v="1"/>
+    <x v="11"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31040000"/>
+    <x v="40"/>
+    <x v="40"/>
+    <x v="40"/>
+    <x v="40"/>
+    <x v="1"/>
+    <x v="12"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30020000"/>
+    <x v="41"/>
+    <x v="41"/>
+    <x v="41"/>
+    <x v="41"/>
+    <x v="1"/>
+    <x v="12"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30150000"/>
+    <x v="42"/>
+    <x v="42"/>
+    <x v="42"/>
+    <x v="42"/>
+    <x v="1"/>
+    <x v="12"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31310000"/>
+    <x v="43"/>
+    <x v="43"/>
+    <x v="43"/>
+    <x v="43"/>
+    <x v="1"/>
+    <x v="12"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30100000"/>
+    <x v="44"/>
+    <x v="44"/>
+    <x v="44"/>
+    <x v="44"/>
+    <x v="2"/>
+    <x v="13"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30220000"/>
+    <x v="45"/>
+    <x v="45"/>
+    <x v="45"/>
+    <x v="45"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30410000"/>
+    <x v="46"/>
+    <x v="46"/>
+    <x v="46"/>
+    <x v="46"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30480000"/>
+    <x v="47"/>
+    <x v="47"/>
+    <x v="47"/>
+    <x v="47"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30710000"/>
+    <x v="48"/>
+    <x v="48"/>
+    <x v="48"/>
+    <x v="48"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31140000"/>
+    <x v="49"/>
+    <x v="49"/>
+    <x v="49"/>
+    <x v="49"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31190000"/>
+    <x v="50"/>
+    <x v="50"/>
+    <x v="50"/>
+    <x v="50"/>
+    <x v="2"/>
+    <x v="14"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31210000"/>
+    <x v="51"/>
+    <x v="51"/>
+    <x v="51"/>
+    <x v="51"/>
+    <x v="2"/>
+    <x v="14"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30240000"/>
+    <x v="52"/>
+    <x v="52"/>
+    <x v="52"/>
+    <x v="52"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30730000"/>
+    <x v="53"/>
+    <x v="53"/>
+    <x v="53"/>
+    <x v="53"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30900000"/>
+    <x v="54"/>
+    <x v="54"/>
+    <x v="54"/>
+    <x v="54"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30260000"/>
+    <x v="55"/>
+    <x v="55"/>
+    <x v="55"/>
+    <x v="55"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30530000"/>
+    <x v="56"/>
+    <x v="56"/>
+    <x v="56"/>
+    <x v="56"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30800000"/>
+    <x v="57"/>
+    <x v="57"/>
+    <x v="57"/>
+    <x v="57"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31030000"/>
+    <x v="58"/>
+    <x v="58"/>
+    <x v="58"/>
+    <x v="58"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31100000"/>
+    <x v="59"/>
+    <x v="59"/>
+    <x v="59"/>
+    <x v="59"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31270000"/>
+    <x v="60"/>
+    <x v="60"/>
+    <x v="60"/>
+    <x v="60"/>
+    <x v="2"/>
+    <x v="15"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30110000"/>
+    <x v="61"/>
+    <x v="61"/>
+    <x v="61"/>
+    <x v="61"/>
+    <x v="2"/>
+    <x v="16"/>
+    <s v="Worth?"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30200000"/>
+    <x v="62"/>
+    <x v="62"/>
+    <x v="62"/>
+    <x v="62"/>
+    <x v="2"/>
+    <x v="16"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="20060000"/>
+    <x v="63"/>
+    <x v="63"/>
+    <x v="63"/>
+    <x v="63"/>
+    <x v="2"/>
+    <x v="17"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30340000"/>
+    <x v="64"/>
+    <x v="64"/>
+    <x v="64"/>
+    <x v="64"/>
+    <x v="1"/>
+    <x v="18"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30050000"/>
+    <x v="65"/>
+    <x v="65"/>
+    <x v="65"/>
+    <x v="65"/>
+    <x v="1"/>
+    <x v="18"/>
+    <s v="OUT"/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="31240000"/>
+    <x v="66"/>
+    <x v="66"/>
+    <x v="66"/>
+    <x v="66"/>
+    <x v="1"/>
+    <x v="18"/>
+    <m/>
+    <n v="2019"/>
+  </r>
+  <r>
+    <n v="30690000"/>
+    <x v="67"/>
+    <x v="67"/>
+    <x v="67"/>
+    <x v="67"/>
+    <x v="2"/>
+    <x v="19"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30250000"/>
+    <x v="68"/>
+    <x v="68"/>
+    <x v="68"/>
+    <x v="68"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30120000"/>
+    <x v="69"/>
+    <x v="69"/>
+    <x v="69"/>
+    <x v="69"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30180000"/>
+    <x v="70"/>
+    <x v="70"/>
+    <x v="70"/>
+    <x v="70"/>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30500000"/>
+    <x v="71"/>
+    <x v="71"/>
+    <x v="71"/>
+    <x v="71"/>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30560000"/>
+    <x v="72"/>
+    <x v="72"/>
+    <x v="72"/>
+    <x v="72"/>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30570000"/>
+    <x v="73"/>
+    <x v="73"/>
+    <x v="73"/>
+    <x v="73"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30585000"/>
+    <x v="74"/>
+    <x v="74"/>
+    <x v="74"/>
+    <x v="74"/>
+    <x v="2"/>
+    <x v="20"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30610000"/>
+    <x v="75"/>
+    <x v="75"/>
+    <x v="75"/>
+    <x v="75"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30640000"/>
+    <x v="76"/>
+    <x v="76"/>
+    <x v="76"/>
+    <x v="76"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30660000"/>
+    <x v="77"/>
+    <x v="77"/>
+    <x v="77"/>
+    <x v="77"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30670000"/>
+    <x v="78"/>
+    <x v="78"/>
+    <x v="78"/>
+    <x v="78"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30720000"/>
+    <x v="79"/>
+    <x v="79"/>
+    <x v="79"/>
+    <x v="79"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30760000"/>
+    <x v="80"/>
+    <x v="80"/>
+    <x v="80"/>
+    <x v="80"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31250000"/>
+    <x v="81"/>
+    <x v="81"/>
+    <x v="81"/>
+    <x v="81"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31300000"/>
+    <x v="82"/>
+    <x v="82"/>
+    <x v="82"/>
+    <x v="82"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31320000"/>
+    <x v="83"/>
+    <x v="83"/>
+    <x v="83"/>
+    <x v="83"/>
+    <x v="2"/>
+    <x v="20"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30920000"/>
+    <x v="84"/>
+    <x v="84"/>
+    <x v="84"/>
+    <x v="84"/>
+    <x v="2"/>
+    <x v="21"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30940000"/>
+    <x v="85"/>
+    <x v="85"/>
+    <x v="85"/>
+    <x v="85"/>
+    <x v="2"/>
+    <x v="22"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30950000"/>
+    <x v="86"/>
+    <x v="86"/>
+    <x v="86"/>
+    <x v="86"/>
+    <x v="2"/>
+    <x v="22"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30540000"/>
+    <x v="87"/>
+    <x v="87"/>
+    <x v="87"/>
+    <x v="87"/>
+    <x v="2"/>
+    <x v="23"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30970000"/>
+    <x v="88"/>
+    <x v="88"/>
+    <x v="88"/>
+    <x v="88"/>
+    <x v="2"/>
+    <x v="23"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30980000"/>
+    <x v="89"/>
+    <x v="89"/>
+    <x v="89"/>
+    <x v="89"/>
+    <x v="2"/>
+    <x v="23"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30990000"/>
+    <x v="90"/>
+    <x v="90"/>
+    <x v="90"/>
+    <x v="90"/>
+    <x v="2"/>
+    <x v="23"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30070000"/>
+    <x v="91"/>
+    <x v="91"/>
+    <x v="91"/>
+    <x v="91"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30090000"/>
+    <x v="92"/>
+    <x v="92"/>
+    <x v="92"/>
+    <x v="92"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30130000"/>
+    <x v="93"/>
+    <x v="93"/>
+    <x v="93"/>
+    <x v="93"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30140000"/>
+    <x v="94"/>
+    <x v="94"/>
+    <x v="94"/>
+    <x v="94"/>
+    <x v="2"/>
+    <x v="24"/>
+    <s v="Riverside"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30420000"/>
+    <x v="95"/>
+    <x v="95"/>
+    <x v="95"/>
+    <x v="95"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30550000"/>
+    <x v="96"/>
+    <x v="96"/>
+    <x v="96"/>
+    <x v="96"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30750000"/>
+    <x v="97"/>
+    <x v="97"/>
+    <x v="97"/>
+    <x v="97"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30770000"/>
+    <x v="98"/>
+    <x v="98"/>
+    <x v="98"/>
+    <x v="98"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31230000"/>
+    <x v="99"/>
+    <x v="99"/>
+    <x v="99"/>
+    <x v="99"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31290000"/>
+    <x v="100"/>
+    <x v="100"/>
+    <x v="100"/>
+    <x v="100"/>
+    <x v="2"/>
+    <x v="24"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30400000"/>
+    <x v="101"/>
+    <x v="101"/>
+    <x v="101"/>
+    <x v="101"/>
+    <x v="2"/>
+    <x v="25"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30440000"/>
+    <x v="102"/>
+    <x v="102"/>
+    <x v="102"/>
+    <x v="102"/>
+    <x v="2"/>
+    <x v="25"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30740000"/>
+    <x v="103"/>
+    <x v="103"/>
+    <x v="103"/>
+    <x v="103"/>
+    <x v="2"/>
+    <x v="25"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30930000"/>
+    <x v="104"/>
+    <x v="104"/>
+    <x v="104"/>
+    <x v="104"/>
+    <x v="2"/>
+    <x v="25"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31000000"/>
+    <x v="105"/>
+    <x v="105"/>
+    <x v="105"/>
+    <x v="105"/>
+    <x v="2"/>
+    <x v="25"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31050000"/>
+    <x v="106"/>
+    <x v="106"/>
+    <x v="106"/>
+    <x v="106"/>
+    <x v="2"/>
+    <x v="25"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31280000"/>
+    <x v="107"/>
+    <x v="107"/>
+    <x v="107"/>
+    <x v="107"/>
+    <x v="2"/>
+    <x v="25"/>
+    <s v="OUT"/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31060000"/>
+    <x v="108"/>
+    <x v="108"/>
+    <x v="108"/>
+    <x v="108"/>
+    <x v="2"/>
+    <x v="26"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30860000"/>
+    <x v="109"/>
+    <x v="109"/>
+    <x v="109"/>
+    <x v="109"/>
+    <x v="2"/>
+    <x v="27"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31090000"/>
+    <x v="110"/>
+    <x v="110"/>
+    <x v="110"/>
+    <x v="110"/>
+    <x v="2"/>
+    <x v="27"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30160000"/>
+    <x v="111"/>
+    <x v="111"/>
+    <x v="111"/>
+    <x v="111"/>
+    <x v="2"/>
+    <x v="28"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30060000"/>
+    <x v="112"/>
+    <x v="112"/>
+    <x v="112"/>
+    <x v="112"/>
+    <x v="2"/>
+    <x v="28"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30430000"/>
+    <x v="113"/>
+    <x v="113"/>
+    <x v="113"/>
+    <x v="113"/>
+    <x v="2"/>
+    <x v="28"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31220000"/>
+    <x v="114"/>
+    <x v="114"/>
+    <x v="114"/>
+    <x v="114"/>
+    <x v="2"/>
+    <x v="28"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30190000"/>
+    <x v="115"/>
+    <x v="115"/>
+    <x v="115"/>
+    <x v="115"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30510000"/>
+    <x v="116"/>
+    <x v="116"/>
+    <x v="116"/>
+    <x v="116"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30170000"/>
+    <x v="117"/>
+    <x v="117"/>
+    <x v="117"/>
+    <x v="117"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30300000"/>
+    <x v="118"/>
+    <x v="118"/>
+    <x v="118"/>
+    <x v="118"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30310000"/>
+    <x v="119"/>
+    <x v="119"/>
+    <x v="119"/>
+    <x v="119"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30330000"/>
+    <x v="120"/>
+    <x v="120"/>
+    <x v="120"/>
+    <x v="120"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30600000"/>
+    <x v="121"/>
+    <x v="121"/>
+    <x v="121"/>
+    <x v="121"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30680000"/>
+    <x v="122"/>
+    <x v="122"/>
+    <x v="122"/>
+    <x v="122"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31020000"/>
+    <x v="123"/>
+    <x v="123"/>
+    <x v="123"/>
+    <x v="123"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31080000"/>
+    <x v="124"/>
+    <x v="124"/>
+    <x v="124"/>
+    <x v="124"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31200000"/>
+    <x v="125"/>
+    <x v="125"/>
+    <x v="125"/>
+    <x v="125"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31260000"/>
+    <x v="126"/>
+    <x v="126"/>
+    <x v="126"/>
+    <x v="126"/>
+    <x v="2"/>
+    <x v="29"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30590000"/>
+    <x v="127"/>
+    <x v="127"/>
+    <x v="127"/>
+    <x v="127"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30010000"/>
+    <x v="128"/>
+    <x v="128"/>
+    <x v="128"/>
+    <x v="128"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30230000"/>
+    <x v="129"/>
+    <x v="129"/>
+    <x v="129"/>
+    <x v="129"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30390000"/>
+    <x v="130"/>
+    <x v="130"/>
+    <x v="130"/>
+    <x v="130"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30780000"/>
+    <x v="131"/>
+    <x v="131"/>
+    <x v="131"/>
+    <x v="131"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="30910000"/>
+    <x v="132"/>
+    <x v="132"/>
+    <x v="132"/>
+    <x v="132"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+  <r>
+    <n v="31350000"/>
+    <x v="133"/>
+    <x v="20"/>
+    <x v="133"/>
+    <x v="133"/>
+    <x v="2"/>
+    <x v="30"/>
+    <m/>
+    <n v="2020"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B87FB73-5E5B-4C64-8111-F9E15E4E82E7}" name="PivotTable4" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C34" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="135">
+        <item x="44"/>
+        <item x="61"/>
+        <item x="111"/>
+        <item x="115"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="52"/>
+        <item x="68"/>
+        <item x="14"/>
+        <item x="64"/>
+        <item x="7"/>
+        <item x="116"/>
+        <item x="87"/>
+        <item x="127"/>
+        <item x="53"/>
+        <item x="8"/>
+        <item x="54"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="15"/>
+        <item x="40"/>
+        <item x="33"/>
+        <item x="63"/>
+        <item x="128"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="65"/>
+        <item x="112"/>
+        <item x="91"/>
+        <item x="9"/>
+        <item x="92"/>
+        <item x="69"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="42"/>
+        <item x="117"/>
+        <item x="70"/>
+        <item x="62"/>
+        <item x="129"/>
+        <item x="55"/>
+        <item x="34"/>
+        <item x="26"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="3"/>
+        <item x="120"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="130"/>
+        <item x="101"/>
+        <item x="46"/>
+        <item x="95"/>
+        <item x="113"/>
+        <item x="102"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="27"/>
+        <item x="47"/>
+        <item x="21"/>
+        <item x="71"/>
+        <item x="31"/>
+        <item x="56"/>
+        <item x="96"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="37"/>
+        <item x="74"/>
+        <item x="121"/>
+        <item x="75"/>
+        <item x="35"/>
+        <item x="76"/>
+        <item x="18"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="122"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="48"/>
+        <item x="79"/>
+        <item x="103"/>
+        <item x="97"/>
+        <item x="80"/>
+        <item x="98"/>
+        <item x="131"/>
+        <item x="57"/>
+        <item x="23"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="109"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="132"/>
+        <item x="84"/>
+        <item x="104"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="36"/>
+        <item x="90"/>
+        <item x="105"/>
+        <item x="123"/>
+        <item x="58"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="12"/>
+        <item x="124"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="49"/>
+        <item x="39"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="50"/>
+        <item x="125"/>
+        <item x="51"/>
+        <item x="114"/>
+        <item x="99"/>
+        <item x="66"/>
+        <item x="81"/>
+        <item x="126"/>
+        <item x="60"/>
+        <item x="107"/>
+        <item x="100"/>
+        <item x="82"/>
+        <item x="43"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="133"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="134">
+        <item x="128"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="65"/>
+        <item x="112"/>
+        <item x="91"/>
+        <item x="9"/>
+        <item x="92"/>
+        <item x="44"/>
+        <item x="61"/>
+        <item x="69"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="42"/>
+        <item x="111"/>
+        <item x="117"/>
+        <item x="70"/>
+        <item x="115"/>
+        <item x="62"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="129"/>
+        <item x="63"/>
+        <item x="52"/>
+        <item x="68"/>
+        <item x="55"/>
+        <item x="34"/>
+        <item x="26"/>
+        <item x="14"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="3"/>
+        <item x="120"/>
+        <item x="64"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="130"/>
+        <item x="101"/>
+        <item x="46"/>
+        <item x="95"/>
+        <item x="113"/>
+        <item x="102"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="27"/>
+        <item x="47"/>
+        <item x="21"/>
+        <item x="71"/>
+        <item x="116"/>
+        <item x="31"/>
+        <item x="56"/>
+        <item x="87"/>
+        <item x="96"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="37"/>
+        <item x="74"/>
+        <item x="127"/>
+        <item x="121"/>
+        <item x="75"/>
+        <item x="35"/>
+        <item x="76"/>
+        <item x="18"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="122"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="48"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="103"/>
+        <item x="97"/>
+        <item x="80"/>
+        <item x="98"/>
+        <item x="131"/>
+        <item x="57"/>
+        <item x="23"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="8"/>
+        <item x="109"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="132"/>
+        <item x="84"/>
+        <item x="104"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="36"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="105"/>
+        <item x="15"/>
+        <item x="123"/>
+        <item x="58"/>
+        <item x="40"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="12"/>
+        <item x="124"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="33"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="49"/>
+        <item x="39"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="50"/>
+        <item x="125"/>
+        <item x="51"/>
+        <item x="114"/>
+        <item x="99"/>
+        <item x="66"/>
+        <item x="81"/>
+        <item x="126"/>
+        <item x="60"/>
+        <item x="107"/>
+        <item x="100"/>
+        <item x="82"/>
+        <item x="43"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="135">
+        <item x="128"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="65"/>
+        <item x="112"/>
+        <item x="91"/>
+        <item x="9"/>
+        <item x="92"/>
+        <item x="44"/>
+        <item x="61"/>
+        <item x="69"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="42"/>
+        <item x="111"/>
+        <item x="117"/>
+        <item x="70"/>
+        <item x="115"/>
+        <item x="62"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="129"/>
+        <item x="63"/>
+        <item x="52"/>
+        <item x="68"/>
+        <item x="55"/>
+        <item x="34"/>
+        <item x="26"/>
+        <item x="14"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="3"/>
+        <item x="120"/>
+        <item x="64"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="130"/>
+        <item x="101"/>
+        <item x="46"/>
+        <item x="95"/>
+        <item x="113"/>
+        <item x="102"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="27"/>
+        <item x="47"/>
+        <item x="21"/>
+        <item x="71"/>
+        <item x="116"/>
+        <item x="31"/>
+        <item x="56"/>
+        <item x="87"/>
+        <item x="96"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="37"/>
+        <item x="74"/>
+        <item x="127"/>
+        <item x="121"/>
+        <item x="75"/>
+        <item x="35"/>
+        <item x="76"/>
+        <item x="18"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="122"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="48"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="103"/>
+        <item x="97"/>
+        <item x="80"/>
+        <item x="98"/>
+        <item x="131"/>
+        <item x="57"/>
+        <item x="23"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="8"/>
+        <item x="109"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="132"/>
+        <item x="84"/>
+        <item x="104"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="36"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="105"/>
+        <item x="15"/>
+        <item x="123"/>
+        <item x="58"/>
+        <item x="40"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="12"/>
+        <item x="124"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="33"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="49"/>
+        <item x="39"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="50"/>
+        <item x="125"/>
+        <item x="51"/>
+        <item x="114"/>
+        <item x="99"/>
+        <item x="66"/>
+        <item x="81"/>
+        <item x="126"/>
+        <item x="60"/>
+        <item x="107"/>
+        <item x="100"/>
+        <item x="82"/>
+        <item x="43"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="133"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="135">
+        <item x="128"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="65"/>
+        <item x="112"/>
+        <item x="91"/>
+        <item x="9"/>
+        <item x="92"/>
+        <item x="44"/>
+        <item x="61"/>
+        <item x="69"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="42"/>
+        <item x="111"/>
+        <item x="117"/>
+        <item x="70"/>
+        <item x="115"/>
+        <item x="62"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="129"/>
+        <item x="63"/>
+        <item x="52"/>
+        <item x="68"/>
+        <item x="55"/>
+        <item x="34"/>
+        <item x="26"/>
+        <item x="14"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="3"/>
+        <item x="120"/>
+        <item x="64"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="130"/>
+        <item x="101"/>
+        <item x="46"/>
+        <item x="95"/>
+        <item x="113"/>
+        <item x="102"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="27"/>
+        <item x="47"/>
+        <item x="21"/>
+        <item x="71"/>
+        <item x="116"/>
+        <item x="31"/>
+        <item x="56"/>
+        <item x="87"/>
+        <item x="96"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="37"/>
+        <item x="74"/>
+        <item x="127"/>
+        <item x="121"/>
+        <item x="75"/>
+        <item x="35"/>
+        <item x="76"/>
+        <item x="18"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="122"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="48"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="103"/>
+        <item x="97"/>
+        <item x="80"/>
+        <item x="98"/>
+        <item x="131"/>
+        <item x="57"/>
+        <item x="23"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="109"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="8"/>
+        <item x="30"/>
+        <item x="54"/>
+        <item x="132"/>
+        <item x="84"/>
+        <item x="104"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="36"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="105"/>
+        <item x="15"/>
+        <item x="123"/>
+        <item x="58"/>
+        <item x="40"/>
+        <item x="106"/>
+        <item x="108"/>
+        <item x="12"/>
+        <item x="124"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="33"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="49"/>
+        <item x="39"/>
+        <item x="13"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="50"/>
+        <item x="125"/>
+        <item x="51"/>
+        <item x="114"/>
+        <item x="99"/>
+        <item x="66"/>
+        <item x="81"/>
+        <item x="126"/>
+        <item x="60"/>
+        <item x="107"/>
+        <item x="100"/>
+        <item x="82"/>
+        <item x="43"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="133"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="32">
+        <item x="1"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="0"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="4"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="10"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="11"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="12"/>
+        <item x="30"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Most recent reassessed" fld="8" subtotal="average" baseField="5" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}" name="Table1" displayName="Table1" ref="A1:I135" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}" name="Table1" displayName="Table1" ref="A1:I135" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:I135" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I135">
     <sortCondition ref="F1:F135"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1F9C6787-AF3E-42F8-88E4-235AC1C1596A}" name="agency_number" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6683F83A-27AA-4C73-8EA3-37CB28F7EE6C}" name="agency_name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F7920334-AB23-48F5-A927-E41C9ED4791F}" name="short_name" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8CA706FA-B778-4359-AA83-9B733DBD6530}" name="clean_name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C98A6C30-D030-444A-A834-9D0C26BFB55B}" name="shpfile_name" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CE881981-CE3C-4963-98DD-50D452D4C1BA}" name="Triad" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{0D872AF7-A538-48C8-BDC8-6BFDCB709A1B}" name="Township" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{322F175E-FB98-49DA-A4B4-17CC4B4D1B43}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1F9C6787-AF3E-42F8-88E4-235AC1C1596A}" name="agency_number" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6683F83A-27AA-4C73-8EA3-37CB28F7EE6C}" name="agency_name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F7920334-AB23-48F5-A927-E41C9ED4791F}" name="short_name" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8CA706FA-B778-4359-AA83-9B733DBD6530}" name="clean_name" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C98A6C30-D030-444A-A834-9D0C26BFB55B}" name="shpfile_name" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CE881981-CE3C-4963-98DD-50D452D4C1BA}" name="Triad" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{0D872AF7-A538-48C8-BDC8-6BFDCB709A1B}" name="Township" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{322F175E-FB98-49DA-A4B4-17CC4B4D1B43}" name="Column1" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{7A23581C-9018-4600-9D8B-3365A7E257E5}" name="Most recent reassessed"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1908,8 +4750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78B4136-5499-4584-8CDE-B5921A95B643}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="I45" sqref="I19:I45"/>
+    <sheetView tabSelected="1" topLeftCell="D94" zoomScale="102" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" x14ac:dyDescent="0.8"/>
@@ -2003,6 +4845,9 @@
         <v>295</v>
       </c>
       <c r="H3" s="6"/>
+      <c r="I3">
+        <v>2019</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A4" s="3">
@@ -2027,6 +4872,9 @@
         <v>295</v>
       </c>
       <c r="H4" s="4"/>
+      <c r="I4">
+        <v>2019</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A5" s="5">
@@ -2053,6 +4901,9 @@
       <c r="H5" s="6" t="s">
         <v>425</v>
       </c>
+      <c r="I5">
+        <v>2019</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A6" s="3">
@@ -2076,7 +4927,10 @@
       <c r="G6" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="11"/>
+      <c r="I6">
+        <v>2019</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A7" s="5">
@@ -2101,6 +4955,9 @@
         <v>424</v>
       </c>
       <c r="H7" s="6"/>
+      <c r="I7">
+        <v>2019</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A8" s="5">
@@ -2127,6 +4984,9 @@
       <c r="H8" s="6" t="s">
         <v>394</v>
       </c>
+      <c r="I8">
+        <v>2019</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A9" s="3">
@@ -2151,6 +5011,9 @@
         <v>282</v>
       </c>
       <c r="H9" s="4"/>
+      <c r="I9">
+        <v>2019</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A10" s="5">
@@ -2175,6 +5038,9 @@
         <v>419</v>
       </c>
       <c r="H10" s="6"/>
+      <c r="I10">
+        <v>2019</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A11" s="3">
@@ -2201,6 +5067,9 @@
       <c r="H11" s="4" t="s">
         <v>425</v>
       </c>
+      <c r="I11">
+        <v>2019</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A12" s="3">
@@ -2225,6 +5094,9 @@
         <v>419</v>
       </c>
       <c r="H12" s="4"/>
+      <c r="I12">
+        <v>2019</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A13" s="5">
@@ -2249,6 +5121,9 @@
         <v>419</v>
       </c>
       <c r="H13" s="6"/>
+      <c r="I13">
+        <v>2019</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A14" s="3">
@@ -2273,6 +5148,9 @@
         <v>419</v>
       </c>
       <c r="H14" s="4"/>
+      <c r="I14">
+        <v>2019</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A15" s="3">
@@ -2297,6 +5175,9 @@
         <v>419</v>
       </c>
       <c r="H15" s="4"/>
+      <c r="I15">
+        <v>2019</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A16" s="3">
@@ -2321,6 +5202,9 @@
         <v>411</v>
       </c>
       <c r="H16" s="4"/>
+      <c r="I16">
+        <v>2019</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A17" s="5">
@@ -2345,6 +5229,9 @@
         <v>411</v>
       </c>
       <c r="H17" s="6"/>
+      <c r="I17">
+        <v>2019</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A18" s="5">
@@ -2371,6 +5258,9 @@
       <c r="H18" s="6" t="s">
         <v>426</v>
       </c>
+      <c r="I18">
+        <v>2019</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A19" s="3">
@@ -3761,6 +6651,9 @@
         <v>343</v>
       </c>
       <c r="H69" s="4"/>
+      <c r="I69">
+        <v>2020</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A70" s="5">
@@ -5567,4 +8460,386 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0CAC8E-01F2-4C07-820A-9300B90359BA}">
+  <dimension ref="A3:C34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B4:B34"/>
+      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" dimension="1" activeRow="28" activeCol="1" previousRow="28" previousCol="1" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+          <references count="1">
+            <reference field="6" count="0"/>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.1" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A3" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A4" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A5" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A6" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A7" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A8" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A9" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A10" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A11" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A12" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A13" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A14" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A15" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A16" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A17" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A18" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A19" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A20" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A21" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A22" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A23" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A24" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A25" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A26" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A27" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A28" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A29" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A30" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C30" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A31" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C31" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A32" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C32" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A33" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A34" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>